<commit_message>
Nature Tower Design Base
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Enemy.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Enemy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3AAD4D-5B7B-44E9-95BC-E02F66972A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD81B109-773E-4D7B-A4D2-E12AD98949E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26520" yWindow="5820" windowWidth="19485" windowHeight="12165" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-27240" yWindow="6210" windowWidth="19425" windowHeight="12165" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRE" sheetId="6" r:id="rId1"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.5,0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pixelperunit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -101,6 +97,9 @@
   <si>
     <t>풀슬라임,NATURE SLIME</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5,0.0625</t>
   </si>
 </sst>
 </file>
@@ -475,7 +474,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -496,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -505,10 +504,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -520,7 +519,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -528,7 +527,7 @@
         <v>2000000</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -553,7 +552,7 @@
         <v>/Sprites/Enemy/2000000/</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1">
         <v>36</v>
@@ -582,7 +581,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -603,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -612,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -627,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -635,7 +634,7 @@
         <v>2010000</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -660,7 +659,7 @@
         <v>/Sprites/Enemy/2010000/</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1">
         <v>36</v>
@@ -686,7 +685,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -707,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -716,10 +715,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -731,7 +730,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -739,7 +738,7 @@
         <v>2020000</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -764,7 +763,7 @@
         <v>/Sprites/Enemy/2020000/</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1">
         <v>36</v>

</xml_diff>

<commit_message>
Adjust Tilmmap, Unit PPU
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Enemy.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Enemy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4232BC01-0B62-40DB-8BC8-D1B8614F7184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45BAA67-7931-4929-A894-EC23DA7F0959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,10 +64,6 @@
   </si>
   <si>
     <t>pivot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pixelperunit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -530,7 +526,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -551,19 +547,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -574,16 +570,14 @@
       <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2000000</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -608,10 +602,7 @@
         <v>/Sprites/Enemy/2000000/</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -619,7 +610,7 @@
         <v>2000100</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -644,10 +635,7 @@
         <v>/Sprites/Enemy/2000100/</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -655,7 +643,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{1F15BD78-2C76-416A-AA9B-FA64F5D504AF}">
       <formula1>COUNTIF(A:A,A1)=1</formula1>
     </dataValidation>
@@ -670,7 +658,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -691,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -700,10 +688,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -714,16 +702,14 @@
       <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2010000</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -748,10 +734,7 @@
         <v>/Sprites/Enemy/2010000/</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -759,7 +742,7 @@
         <v>2010100</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -784,10 +767,7 @@
         <v>/Sprites/Enemy/2010100/</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -810,7 +790,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -831,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -840,10 +820,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -854,16 +834,14 @@
       <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2020000</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -888,10 +866,7 @@
         <v>/Sprites/Enemy/2020000/</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -899,7 +874,7 @@
         <v>2020001</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -924,10 +899,7 @@
         <v>/Sprites/Enemy/2020001/</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -935,7 +907,7 @@
         <v>2020002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -960,10 +932,7 @@
         <v>/Sprites/Enemy/2020002/</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -971,7 +940,7 @@
         <v>2021002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -996,10 +965,7 @@
         <v>/Sprites/Enemy/2021002/</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -1007,7 +973,7 @@
         <v>2021003</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1032,10 +998,7 @@
         <v>/Sprites/Enemy/2021003/</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1043,7 +1006,7 @@
         <v>2021004</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1068,10 +1031,7 @@
         <v>/Sprites/Enemy/2021004/</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1079,7 +1039,7 @@
         <v>2022005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1104,10 +1064,7 @@
         <v>/Sprites/Enemy/2022005/</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1115,7 +1072,7 @@
         <v>2020100</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1140,10 +1097,7 @@
         <v>/Sprites/Enemy/2020100/</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1151,7 +1105,7 @@
         <v>2020101</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1176,10 +1130,7 @@
         <v>/Sprites/Enemy/2020101/</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="1">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1187,7 +1138,7 @@
         <v>2020102</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1212,10 +1163,7 @@
         <v>/Sprites/Enemy/2020102/</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1223,7 +1171,7 @@
         <v>2021102</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1248,10 +1196,7 @@
         <v>/Sprites/Enemy/2021102/</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1259,7 +1204,7 @@
         <v>2021103</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1284,10 +1229,7 @@
         <v>/Sprites/Enemy/2021103/</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1295,7 +1237,7 @@
         <v>2021104</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1320,10 +1262,7 @@
         <v>/Sprites/Enemy/2021104/</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="1">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1331,7 +1270,7 @@
         <v>2022105</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1356,10 +1295,7 @@
         <v>/Sprites/Enemy/2022105/</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>